<commit_message>
processed some more results
</commit_message>
<xml_diff>
--- a/scaling-plots/excel-processed/erase_create_cluster.xlsx
+++ b/scaling-plots/excel-processed/erase_create_cluster.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t xml:space="preserve">#n iters</t>
   </si>
@@ -106,16 +106,31 @@
     <t xml:space="preserve">% step 8</t>
   </si>
   <si>
-    <t xml:space="preserve">total scaling</t>
+    <t xml:space="preserve">speedup</t>
   </si>
   <si>
-    <t xml:space="preserve">scaling step 2scaling step 3</t>
+    <t xml:space="preserve">speedup step 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">speedup step 3</t>
   </si>
   <si>
     <t xml:space="preserve"># obj per thread</t>
   </si>
   <si>
     <t xml:space="preserve"># obj scaling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max speedup index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#N thread</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#N object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execution time</t>
   </si>
   <si>
     <t xml:space="preserve">ref. Time</t>
@@ -156,7 +171,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -177,6 +192,21 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -253,7 +283,1552 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFD320"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>execution time and number of object
+erase create</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.328437105300089"/>
+          <c:y val="0.0674157303370787"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AM$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#N object</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AK$5:$AK$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1584</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1476</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1368</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1260</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1152</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1044</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>936</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>828</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>648</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AM$5:$AM$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>9009470</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9009476</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9009474</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9009475</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9009471</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9009466</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9009470</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9009469</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9009472</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9009475</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9009472</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9009471</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9009470</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9009471</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9009474</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9013336</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8991035</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4587192</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2052738</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="3029090"/>
+        <c:axId val="21585908"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AN$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Execution time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AK$5:$AK$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1584</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1476</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1368</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1260</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1152</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1044</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>936</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>828</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>648</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AN$5:$AN$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>11.49039</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.844622</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.249342</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.671851</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.776621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.796471</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.930823</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.005428</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.39012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.264253</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.925571</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.033217</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26.516059</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30.790395</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>37.496086</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>48.474888</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>70.500746</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>71.210804</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>77.99197</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="14823101"/>
+        <c:axId val="75683018"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="3029090"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>#N thread</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="21585908"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="21585908"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>#N object</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="3029090"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="14823101"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="75683018"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="75683018"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Execution time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="14823101"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>execution time and speedup
+erase create</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.328530663797539"/>
+          <c:y val="0.0676077979448766"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AL$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>speedup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AK$5:$AK$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1584</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1476</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1368</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1260</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1152</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1044</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>936</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>828</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>648</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AL$5:$AL$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>6.78758249284837</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.58458919161793</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3670334292242</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.97656403190663</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.66118281108263</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.27098454759922</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.89566483790574</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.89854043612564</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.24097123890437</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.04853331193273</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.72711310960164</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.24517396068949</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.9413107732186</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.53299673485839</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.08000296350931</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.60891490868427</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.10625737208511</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.09522664566461</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="84553740"/>
+        <c:axId val="60166161"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AN$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Execution time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AK$5:$AK$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1584</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1476</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1368</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1260</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1152</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1044</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>936</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>828</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>648</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AN$5:$AN$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>11.49039</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.844622</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.249342</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.671851</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.776621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.796471</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.930823</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.005428</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.39012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.264253</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.925571</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.033217</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26.516059</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30.790395</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>37.496086</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>48.474888</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>70.500746</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>71.210804</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>77.99197</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="41505330"/>
+        <c:axId val="22406077"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="84553740"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>#N thread</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="60166161"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="60166161"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>#N object</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="84553740"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="41505330"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="22406077"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="22406077"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Execution time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="41505330"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>617400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>133920</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>28440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="34216920" y="669240"/>
+        <a:ext cx="7695360" cy="3748320"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>628920</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>145440</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>86040</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="34228440" y="4628160"/>
+        <a:ext cx="7695360" cy="3748320"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -261,13 +1836,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG121"/>
+  <dimension ref="A1:AN121"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AN39" activeCellId="0" sqref="AN39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="13.34"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -370,11 +1951,29 @@
       <c r="AC4" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="AD4" s="0" t="s">
+        <v>30</v>
+      </c>
       <c r="AF4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="AI4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN4" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -480,6 +2079,26 @@
         <f aca="false">AF$118 / AF5</f>
         <v>10.0706800497654</v>
       </c>
+      <c r="AI5" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB5:AB10), AB5:AB10) + 4</f>
+        <v>10</v>
+      </c>
+      <c r="AK5" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI5)</f>
+        <v>1584</v>
+      </c>
+      <c r="AL5" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI5)</f>
+        <v>6.78758249284837</v>
+      </c>
+      <c r="AM5" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI5)</f>
+        <v>9009470</v>
+      </c>
+      <c r="AN5" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI5)</f>
+        <v>11.49039</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -584,6 +2203,26 @@
         <f aca="false">AF$118 / AF6</f>
         <v>10.0706811675534</v>
       </c>
+      <c r="AI6" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB11:AB16), AB11:AB16) + 10</f>
+        <v>16</v>
+      </c>
+      <c r="AK6" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI6)</f>
+        <v>1476</v>
+      </c>
+      <c r="AL6" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI6)</f>
+        <v>6.58458919161793</v>
+      </c>
+      <c r="AM6" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI6)</f>
+        <v>9009476</v>
+      </c>
+      <c r="AN6" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI6)</f>
+        <v>11.844622</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -688,6 +2327,26 @@
         <f aca="false">AF$118 / AF7</f>
         <v>10.0706811675534</v>
       </c>
+      <c r="AI7" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB17:AB22), AB17:AB22) + 16</f>
+        <v>22</v>
+      </c>
+      <c r="AK7" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI7)</f>
+        <v>1368</v>
+      </c>
+      <c r="AL7" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI7)</f>
+        <v>6.3670334292242</v>
+      </c>
+      <c r="AM7" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI7)</f>
+        <v>9009474</v>
+      </c>
+      <c r="AN7" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI7)</f>
+        <v>12.249342</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -792,6 +2451,26 @@
         <f aca="false">AF$118 / AF8</f>
         <v>10.0706822853417</v>
       </c>
+      <c r="AI8" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB23:AB28), AB23:AB28) + 22</f>
+        <v>27</v>
+      </c>
+      <c r="AK8" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI8)</f>
+        <v>1260</v>
+      </c>
+      <c r="AL8" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI8)</f>
+        <v>4.97656403190663</v>
+      </c>
+      <c r="AM8" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI8)</f>
+        <v>9009475</v>
+      </c>
+      <c r="AN8" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI8)</f>
+        <v>15.671851</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -896,6 +2575,26 @@
         <f aca="false">AF$118 / AF9</f>
         <v>10.0706766964028</v>
       </c>
+      <c r="AI9" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB29:AB34), AB29:AB34) + 28</f>
+        <v>34</v>
+      </c>
+      <c r="AK9" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI9)</f>
+        <v>1152</v>
+      </c>
+      <c r="AL9" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI9)</f>
+        <v>5.66118281108263</v>
+      </c>
+      <c r="AM9" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI9)</f>
+        <v>9009471</v>
+      </c>
+      <c r="AN9" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI9)</f>
+        <v>13.776621</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -1000,6 +2699,26 @@
         <f aca="false">AF$118 / AF10</f>
         <v>10.0706834031303</v>
       </c>
+      <c r="AI10" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB35:AB40), AB35:AB40) + 34</f>
+        <v>40</v>
+      </c>
+      <c r="AK10" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI10)</f>
+        <v>1044</v>
+      </c>
+      <c r="AL10" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI10)</f>
+        <v>5.27098454759922</v>
+      </c>
+      <c r="AM10" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI10)</f>
+        <v>9009466</v>
+      </c>
+      <c r="AN10" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI10)</f>
+        <v>14.796471</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -1104,6 +2823,26 @@
         <f aca="false">AF$118 / AF11</f>
         <v>9.38404589837138</v>
       </c>
+      <c r="AI11" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB41:AB46), AB41:AB46) + 40</f>
+        <v>46</v>
+      </c>
+      <c r="AK11" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI11)</f>
+        <v>936</v>
+      </c>
+      <c r="AL11" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI11)</f>
+        <v>4.89566483790574</v>
+      </c>
+      <c r="AM11" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI11)</f>
+        <v>9009470</v>
+      </c>
+      <c r="AN11" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI11)</f>
+        <v>15.930823</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -1208,6 +2947,26 @@
         <f aca="false">AF$118 / AF12</f>
         <v>9.38403964892076</v>
       </c>
+      <c r="AI12" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB47:AB52), AB47:AB52) + 46</f>
+        <v>52</v>
+      </c>
+      <c r="AK12" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI12)</f>
+        <v>828</v>
+      </c>
+      <c r="AL12" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI12)</f>
+        <v>3.89854043612564</v>
+      </c>
+      <c r="AM12" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI12)</f>
+        <v>9009469</v>
+      </c>
+      <c r="AN12" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI12)</f>
+        <v>20.005428</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -1312,6 +3071,26 @@
         <f aca="false">AF$118 / AF13</f>
         <v>9.38404277364503</v>
       </c>
+      <c r="AI13" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB53:AB58), AB53:AB58) + 52</f>
+        <v>57</v>
+      </c>
+      <c r="AK13" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI13)</f>
+        <v>720</v>
+      </c>
+      <c r="AL13" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI13)</f>
+        <v>4.24097123890437</v>
+      </c>
+      <c r="AM13" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI13)</f>
+        <v>9009472</v>
+      </c>
+      <c r="AN13" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI13)</f>
+        <v>18.39012</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -1416,6 +3195,26 @@
         <f aca="false">AF$118 / AF14</f>
         <v>9.38404069049528</v>
       </c>
+      <c r="AI14" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB59:AB64), AB59:AB64) + 58</f>
+        <v>64</v>
+      </c>
+      <c r="AK14" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI14)</f>
+        <v>648</v>
+      </c>
+      <c r="AL14" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI14)</f>
+        <v>4.04853331193273</v>
+      </c>
+      <c r="AM14" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI14)</f>
+        <v>9009475</v>
+      </c>
+      <c r="AN14" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI14)</f>
+        <v>19.264253</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -1520,6 +3319,26 @@
         <f aca="false">AF$118 / AF15</f>
         <v>9.3840375657724</v>
       </c>
+      <c r="AI15" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB65:AB70), AB65:AB70) + 64</f>
+        <v>70</v>
+      </c>
+      <c r="AK15" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI15)</f>
+        <v>576</v>
+      </c>
+      <c r="AL15" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI15)</f>
+        <v>3.72711310960164</v>
+      </c>
+      <c r="AM15" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI15)</f>
+        <v>9009472</v>
+      </c>
+      <c r="AN15" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI15)</f>
+        <v>20.925571</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -1624,6 +3443,26 @@
         <f aca="false">AF$118 / AF16</f>
         <v>9.38403964892076</v>
       </c>
+      <c r="AI16" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB71:AB76), AB71:AB76) + 70</f>
+        <v>75</v>
+      </c>
+      <c r="AK16" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI16)</f>
+        <v>504</v>
+      </c>
+      <c r="AL16" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI16)</f>
+        <v>3.24517396068949</v>
+      </c>
+      <c r="AM16" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI16)</f>
+        <v>9009471</v>
+      </c>
+      <c r="AN16" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI16)</f>
+        <v>24.033217</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -1728,6 +3567,26 @@
         <f aca="false">AF$118 / AF17</f>
         <v>8.69740549752466</v>
       </c>
+      <c r="AI17" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB77:AB82), AB77:AB82) + 76</f>
+        <v>82</v>
+      </c>
+      <c r="AK17" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI17)</f>
+        <v>432</v>
+      </c>
+      <c r="AL17" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI17)</f>
+        <v>2.9413107732186</v>
+      </c>
+      <c r="AM17" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI17)</f>
+        <v>9009470</v>
+      </c>
+      <c r="AN17" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI17)</f>
+        <v>26.516059</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -1832,6 +3691,26 @@
         <f aca="false">AF$118 / AF18</f>
         <v>8.69740742824967</v>
       </c>
+      <c r="AI18" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB83:AB88), AB83:AB88) + 82</f>
+        <v>88</v>
+      </c>
+      <c r="AK18" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI18)</f>
+        <v>360</v>
+      </c>
+      <c r="AL18" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI18)</f>
+        <v>2.53299673485839</v>
+      </c>
+      <c r="AM18" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI18)</f>
+        <v>9009471</v>
+      </c>
+      <c r="AN18" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI18)</f>
+        <v>30.790395</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -1936,6 +3815,26 @@
         <f aca="false">AF$118 / AF19</f>
         <v>8.69740067071588</v>
       </c>
+      <c r="AI19" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB89:AB94), AB89:AB94) + 88</f>
+        <v>94</v>
+      </c>
+      <c r="AK19" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI19)</f>
+        <v>288</v>
+      </c>
+      <c r="AL19" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI19)</f>
+        <v>2.08000296350931</v>
+      </c>
+      <c r="AM19" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI19)</f>
+        <v>9009474</v>
+      </c>
+      <c r="AN19" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI19)</f>
+        <v>37.496086</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -2040,6 +3939,26 @@
         <f aca="false">AF$118 / AF20</f>
         <v>8.69740646288706</v>
       </c>
+      <c r="AI20" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB95:AB100), AB95:AB100) + 94</f>
+        <v>100</v>
+      </c>
+      <c r="AK20" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI20)</f>
+        <v>216</v>
+      </c>
+      <c r="AL20" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI20)</f>
+        <v>1.60891490868427</v>
+      </c>
+      <c r="AM20" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI20)</f>
+        <v>9013336</v>
+      </c>
+      <c r="AN20" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI20)</f>
+        <v>48.474888</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -2144,6 +4063,26 @@
         <f aca="false">AF$118 / AF21</f>
         <v>8.6974083936125</v>
       </c>
+      <c r="AI21" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB101:AB106), AB101:AB106) + 101</f>
+        <v>105</v>
+      </c>
+      <c r="AK21" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI21)</f>
+        <v>144</v>
+      </c>
+      <c r="AL21" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI21)</f>
+        <v>1.10625737208511</v>
+      </c>
+      <c r="AM21" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI21)</f>
+        <v>8991035</v>
+      </c>
+      <c r="AN21" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI21)</f>
+        <v>70.500746</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -2248,6 +4187,26 @@
         <f aca="false">AF$118 / AF22</f>
         <v>8.69740453216248</v>
       </c>
+      <c r="AI22" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB107:AB112), AB107:AB112) + 106</f>
+        <v>112</v>
+      </c>
+      <c r="AK22" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI22)</f>
+        <v>72</v>
+      </c>
+      <c r="AL22" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI22)</f>
+        <v>1.09522664566461</v>
+      </c>
+      <c r="AM22" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI22)</f>
+        <v>4587192</v>
+      </c>
+      <c r="AN22" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI22)</f>
+        <v>71.210804</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -2352,6 +4311,26 @@
         <f aca="false">AF$118 / AF23</f>
         <v>8.01077088885362</v>
       </c>
+      <c r="AI23" s="0" t="n">
+        <f aca="false"> MATCH(MAX(AB113:AB118), AB113:AB118) + 112</f>
+        <v>117</v>
+      </c>
+      <c r="AK23" s="0" t="n">
+        <f aca="false">INDEX(P$1:P$118,$AI23)</f>
+        <v>36</v>
+      </c>
+      <c r="AL23" s="0" t="n">
+        <f aca="false">INDEX(AB$1:AB$118,$AI23)</f>
+        <v>1</v>
+      </c>
+      <c r="AM23" s="0" t="n">
+        <f aca="false">INDEX(D$1:D$118,$AI23)</f>
+        <v>2052738</v>
+      </c>
+      <c r="AN23" s="0" t="n">
+        <f aca="false">INDEX(E$1:E$118,$AI23)</f>
+        <v>77.99197</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -12235,34 +14214,34 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E120" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="L120" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="M120" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="N120" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12315,5 +14294,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrected a small error in a legend
</commit_message>
<xml_diff>
--- a/scaling-plots/excel-processed/erase_create_cluster.xlsx
+++ b/scaling-plots/excel-processed/erase_create_cluster.xlsx
@@ -346,7 +346,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -376,8 +376,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.328437105300089"/>
-          <c:y val="0.0674157303370787"/>
+          <c:x val="0.328476017000607"/>
+          <c:y val="0.06732616212063"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -439,6 +439,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -586,8 +587,8 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="3029090"/>
-        <c:axId val="21585908"/>
+        <c:axId val="76340798"/>
+        <c:axId val="74247943"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -638,6 +639,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -785,11 +787,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="14823101"/>
-        <c:axId val="75683018"/>
+        <c:axId val="28472341"/>
+        <c:axId val="28386588"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="3029090"/>
+        <c:axId val="76340798"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -823,7 +825,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -845,12 +847,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21585908"/>
+        <c:crossAx val="74247943"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="21585908"/>
+        <c:axId val="74247943"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -893,7 +895,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -915,12 +917,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3029090"/>
+        <c:crossAx val="76340798"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="14823101"/>
+        <c:axId val="28472341"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -948,11 +950,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75683018"/>
-        <c:crossBetween val="between"/>
+        <c:crossAx val="28386588"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75683018"/>
+        <c:axId val="28386588"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -986,7 +988,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1008,9 +1010,9 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14823101"/>
+        <c:crossAx val="28472341"/>
         <c:crosses val="max"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1056,7 +1058,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1086,8 +1088,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.328530663797539"/>
-          <c:y val="0.0676077979448766"/>
+          <c:x val="0.328569426930083"/>
+          <c:y val="0.0675182481751825"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1149,6 +1151,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1296,8 +1299,8 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="84553740"/>
-        <c:axId val="60166161"/>
+        <c:axId val="86129723"/>
+        <c:axId val="21930925"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1348,6 +1351,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1495,11 +1499,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="41505330"/>
-        <c:axId val="22406077"/>
+        <c:axId val="11681045"/>
+        <c:axId val="3776982"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84553740"/>
+        <c:axId val="86129723"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1533,7 +1537,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1555,12 +1559,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60166161"/>
+        <c:crossAx val="21930925"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60166161"/>
+        <c:axId val="21930925"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1590,7 +1594,7 @@
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>#N object</a:t>
+                  <a:t>speedup</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1603,7 +1607,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1625,12 +1629,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84553740"/>
+        <c:crossAx val="86129723"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41505330"/>
+        <c:axId val="11681045"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1658,11 +1662,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22406077"/>
-        <c:crossBetween val="between"/>
+        <c:crossAx val="3776982"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="22406077"/>
+        <c:axId val="3776982"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1696,7 +1700,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1718,9 +1722,9 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41505330"/>
+        <c:crossAx val="11681045"/>
         <c:crosses val="max"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1777,9 +1781,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>50</xdr:col>
-      <xdr:colOff>133920</xdr:colOff>
+      <xdr:colOff>133560</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>28440</xdr:rowOff>
+      <xdr:rowOff>28080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1787,8 +1791,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="34216920" y="669240"/>
-        <a:ext cx="7695360" cy="3748320"/>
+        <a:off x="34263360" y="669240"/>
+        <a:ext cx="7707600" cy="3747960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1807,9 +1811,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>50</xdr:col>
-      <xdr:colOff>145440</xdr:colOff>
+      <xdr:colOff>145080</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>86040</xdr:rowOff>
+      <xdr:rowOff>85680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1817,8 +1821,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="34228440" y="4628160"/>
-        <a:ext cx="7695360" cy="3748320"/>
+        <a:off x="34274880" y="4628160"/>
+        <a:ext cx="7707600" cy="3747960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1838,16 +1842,16 @@
   </sheetPr>
   <dimension ref="A1:AN121"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AN39" activeCellId="0" sqref="AN39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AF10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AM32" activeCellId="0" sqref="AM32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="13.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2080,7 +2084,7 @@
         <v>10.0706800497654</v>
       </c>
       <c r="AI5" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB5:AB10), AB5:AB10) + 4</f>
+        <f aca="false">MATCH(MAX(AB5:AB10), AB5:AB10) + 4</f>
         <v>10</v>
       </c>
       <c r="AK5" s="0" t="n">
@@ -2204,7 +2208,7 @@
         <v>10.0706811675534</v>
       </c>
       <c r="AI6" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB11:AB16), AB11:AB16) + 10</f>
+        <f aca="false">MATCH(MAX(AB11:AB16), AB11:AB16) + 10</f>
         <v>16</v>
       </c>
       <c r="AK6" s="0" t="n">
@@ -2328,7 +2332,7 @@
         <v>10.0706811675534</v>
       </c>
       <c r="AI7" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB17:AB22), AB17:AB22) + 16</f>
+        <f aca="false">MATCH(MAX(AB17:AB22), AB17:AB22) + 16</f>
         <v>22</v>
       </c>
       <c r="AK7" s="0" t="n">
@@ -2452,7 +2456,7 @@
         <v>10.0706822853417</v>
       </c>
       <c r="AI8" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB23:AB28), AB23:AB28) + 22</f>
+        <f aca="false">MATCH(MAX(AB23:AB28), AB23:AB28) + 22</f>
         <v>27</v>
       </c>
       <c r="AK8" s="0" t="n">
@@ -2576,7 +2580,7 @@
         <v>10.0706766964028</v>
       </c>
       <c r="AI9" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB29:AB34), AB29:AB34) + 28</f>
+        <f aca="false">MATCH(MAX(AB29:AB34), AB29:AB34) + 28</f>
         <v>34</v>
       </c>
       <c r="AK9" s="0" t="n">
@@ -2700,7 +2704,7 @@
         <v>10.0706834031303</v>
       </c>
       <c r="AI10" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB35:AB40), AB35:AB40) + 34</f>
+        <f aca="false">MATCH(MAX(AB35:AB40), AB35:AB40) + 34</f>
         <v>40</v>
       </c>
       <c r="AK10" s="0" t="n">
@@ -2824,7 +2828,7 @@
         <v>9.38404589837138</v>
       </c>
       <c r="AI11" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB41:AB46), AB41:AB46) + 40</f>
+        <f aca="false">MATCH(MAX(AB41:AB46), AB41:AB46) + 40</f>
         <v>46</v>
       </c>
       <c r="AK11" s="0" t="n">
@@ -2948,7 +2952,7 @@
         <v>9.38403964892076</v>
       </c>
       <c r="AI12" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB47:AB52), AB47:AB52) + 46</f>
+        <f aca="false">MATCH(MAX(AB47:AB52), AB47:AB52) + 46</f>
         <v>52</v>
       </c>
       <c r="AK12" s="0" t="n">
@@ -3072,7 +3076,7 @@
         <v>9.38404277364503</v>
       </c>
       <c r="AI13" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB53:AB58), AB53:AB58) + 52</f>
+        <f aca="false">MATCH(MAX(AB53:AB58), AB53:AB58) + 52</f>
         <v>57</v>
       </c>
       <c r="AK13" s="0" t="n">
@@ -3196,7 +3200,7 @@
         <v>9.38404069049528</v>
       </c>
       <c r="AI14" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB59:AB64), AB59:AB64) + 58</f>
+        <f aca="false">MATCH(MAX(AB59:AB64), AB59:AB64) + 58</f>
         <v>64</v>
       </c>
       <c r="AK14" s="0" t="n">
@@ -3320,7 +3324,7 @@
         <v>9.3840375657724</v>
       </c>
       <c r="AI15" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB65:AB70), AB65:AB70) + 64</f>
+        <f aca="false">MATCH(MAX(AB65:AB70), AB65:AB70) + 64</f>
         <v>70</v>
       </c>
       <c r="AK15" s="0" t="n">
@@ -3444,7 +3448,7 @@
         <v>9.38403964892076</v>
       </c>
       <c r="AI16" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB71:AB76), AB71:AB76) + 70</f>
+        <f aca="false">MATCH(MAX(AB71:AB76), AB71:AB76) + 70</f>
         <v>75</v>
       </c>
       <c r="AK16" s="0" t="n">
@@ -3568,7 +3572,7 @@
         <v>8.69740549752466</v>
       </c>
       <c r="AI17" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB77:AB82), AB77:AB82) + 76</f>
+        <f aca="false">MATCH(MAX(AB77:AB82), AB77:AB82) + 76</f>
         <v>82</v>
       </c>
       <c r="AK17" s="0" t="n">
@@ -3692,7 +3696,7 @@
         <v>8.69740742824967</v>
       </c>
       <c r="AI18" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB83:AB88), AB83:AB88) + 82</f>
+        <f aca="false">MATCH(MAX(AB83:AB88), AB83:AB88) + 82</f>
         <v>88</v>
       </c>
       <c r="AK18" s="0" t="n">
@@ -3816,7 +3820,7 @@
         <v>8.69740067071588</v>
       </c>
       <c r="AI19" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB89:AB94), AB89:AB94) + 88</f>
+        <f aca="false">MATCH(MAX(AB89:AB94), AB89:AB94) + 88</f>
         <v>94</v>
       </c>
       <c r="AK19" s="0" t="n">
@@ -3940,7 +3944,7 @@
         <v>8.69740646288706</v>
       </c>
       <c r="AI20" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB95:AB100), AB95:AB100) + 94</f>
+        <f aca="false">MATCH(MAX(AB95:AB100), AB95:AB100) + 94</f>
         <v>100</v>
       </c>
       <c r="AK20" s="0" t="n">
@@ -4064,7 +4068,7 @@
         <v>8.6974083936125</v>
       </c>
       <c r="AI21" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB101:AB106), AB101:AB106) + 101</f>
+        <f aca="false">MATCH(MAX(AB101:AB106), AB101:AB106) + 101</f>
         <v>105</v>
       </c>
       <c r="AK21" s="0" t="n">
@@ -4188,7 +4192,7 @@
         <v>8.69740453216248</v>
       </c>
       <c r="AI22" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB107:AB112), AB107:AB112) + 106</f>
+        <f aca="false">MATCH(MAX(AB107:AB112), AB107:AB112) + 106</f>
         <v>112</v>
       </c>
       <c r="AK22" s="0" t="n">
@@ -4312,7 +4316,7 @@
         <v>8.01077088885362</v>
       </c>
       <c r="AI23" s="0" t="n">
-        <f aca="false"> MATCH(MAX(AB113:AB118), AB113:AB118) + 112</f>
+        <f aca="false">MATCH(MAX(AB113:AB118), AB113:AB118) + 112</f>
         <v>117</v>
       </c>
       <c r="AK23" s="0" t="n">

</xml_diff>